<commit_message>
Updates for Phase 3 Action Items
</commit_message>
<xml_diff>
--- a/Documents/Phase 3/Data Analysis for Neural Network.xlsx
+++ b/Documents/Phase 3/Data Analysis for Neural Network.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11910" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="7">
   <si>
     <t>#</t>
   </si>
@@ -41,16 +42,10 @@
     <t>% of Total</t>
   </si>
   <si>
-    <t>Sum</t>
+    <t>Normal</t>
   </si>
   <si>
-    <t>Average</t>
-  </si>
-  <si>
-    <t>Running Total</t>
-  </si>
-  <si>
-    <t>Count</t>
+    <t>Malicious</t>
   </si>
 </sst>
 </file>
@@ -101,7 +96,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -109,12 +104,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFF7C80"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -880,7 +883,1263 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Accuracy of Neural Network</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:areaChart>
+        <c:grouping val="percentStacked"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$C$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Malicious</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:srgbClr val="FF7C80"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$C$3:$C$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1.1111111111111112E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2222222222222223E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4444444444444446E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5555555555555552E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.7777777777777779E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.8888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.14444444444444443</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.15555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.17777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.18888888888888888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.21111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.23333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.24444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25555555555555554</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.26666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.27777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.28888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.31111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.32222222222222224</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-113E-49D5-8599-9BA8E91C93E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$D$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Normal</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent6">
+                <a:lumMod val="60000"/>
+                <a:lumOff val="40000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$D$3:$D$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>1.1111111111111112E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.2222222222222223E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.3333333333333333E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.4444444444444446E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5.5555555555555552E-2</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7.7777777777777779E-2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.8888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.1</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.1111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.12222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.14444444444444443</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.15555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.16666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.17777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.18888888888888888</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.21111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.23333333333333334</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.24444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.25555555555555554</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.26666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.27777777777777779</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.28888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.3</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.31111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.32222222222222224</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.34444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.35555555555555557</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.36666666666666664</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.37777777777777777</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.3888888888888889</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.41111111111111109</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.42222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.43333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.44444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.45555555555555555</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.46666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.4777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.48888888888888887</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.5</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.51111111111111107</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.52222222222222225</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.53333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.5444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.56666666666666665</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.57777777777777772</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.58888888888888891</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.61111111111111116</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.62222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.6333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.64444444444444449</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.65555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-113E-49D5-8599-9BA8E91C93E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="430950800"/>
+        <c:axId val="430955064"/>
+      </c:areaChart>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$E$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Accuracy</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="75000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$E$3:$E$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.33329999999999999</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.42220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.42220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.42220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.42220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.42220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.42220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.42220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.42220000000000002</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-113E-49D5-8599-9BA8E91C93E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet2!$F$2</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>% of Total</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="34925" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="85000"/>
+                  <a:lumOff val="15000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet2!$F$3:$F$62</c:f>
+              <c:numCache>
+                <c:formatCode>0.00%</c:formatCode>
+                <c:ptCount val="60"/>
+                <c:pt idx="0">
+                  <c:v>2.2222222222222223E-2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>4.4444444444444446E-2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>6.6666666666666666E-2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.8888888888888892E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1111111111111111</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.13333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.15555555555555556</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.17777777777777778</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.2</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>0.22222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.24444444444444444</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>0.26666666666666666</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>0.28888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>0.31111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.33333333333333331</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.35555555555555557</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>0.37777777777777777</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>0.4</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>0.42222222222222222</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.44444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.46666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>0.48888888888888887</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>0.51111111111111107</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>0.53333333333333333</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>0.55555555555555558</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>0.57777777777777772</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>0.6</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>0.62222222222222223</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>0.64444444444444449</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>0.66666666666666663</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>0.67777777777777781</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>0.68888888888888888</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>0.71111111111111103</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>0.72222222222222221</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>0.73333333333333339</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>0.74444444444444446</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>0.75555555555555554</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>0.76666666666666661</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>0.77777777777777768</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>0.78888888888888886</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>0.8</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>0.81111111111111112</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>0.82222222222222219</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.83333333333333326</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>0.84444444444444433</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.85555555555555562</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>0.8666666666666667</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>0.87777777777777777</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>0.88888888888888884</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>0.89999999999999991</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>0.91111111111111098</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>0.92222222222222228</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>0.93333333333333335</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>0.94444444444444442</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>0.95555555555555549</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>0.96666666666666656</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>0.97777777777777786</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>0.98888888888888893</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-113E-49D5-8599-9BA8E91C93E6}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="430950800"/>
+        <c:axId val="430955064"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="430950800"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="430955064"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="430955064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="430950800"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="zero"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1416,20 +2675,568 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="328">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="95000"/>
+              <a:lumOff val="5000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="75000"/>
+              <a:lumOff val="25000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill>
+        <a:gsLst>
+          <a:gs pos="100000">
+            <a:schemeClr val="lt1">
+              <a:lumMod val="85000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="0">
+            <a:schemeClr val="lt1"/>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+      </a:gradFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>114299</xdr:colOff>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>133349</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>104774</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>400050</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
       <xdr:row>23</xdr:row>
       <xdr:rowOff>38100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>47625</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>123825</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1750,8 +3557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B4:F64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+    <sheetView topLeftCell="A30" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4:F64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2861,4 +4668,1238 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="B2:F62"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="W45" sqref="W45"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F2" s="4" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" s="1">
+        <v>1</v>
+      </c>
+      <c r="C3" s="5">
+        <f>B3/90</f>
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="D3" s="5">
+        <f t="shared" ref="D3:D62" si="0">B3/90</f>
+        <v>1.1111111111111112E-2</v>
+      </c>
+      <c r="E3" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F3" s="3">
+        <f>(C3+D3)</f>
+        <v>2.2222222222222223E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" s="1">
+        <v>2</v>
+      </c>
+      <c r="C4" s="5">
+        <f t="shared" ref="C4:C62" si="1">B4/90</f>
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="D4" s="5">
+        <f t="shared" si="0"/>
+        <v>2.2222222222222223E-2</v>
+      </c>
+      <c r="E4" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F4" s="3">
+        <f t="shared" ref="F4:F62" si="2">(C4+D4)</f>
+        <v>4.4444444444444446E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" s="1">
+        <v>3</v>
+      </c>
+      <c r="C5" s="5">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="D5" s="5">
+        <f>B5/90</f>
+        <v>3.3333333333333333E-2</v>
+      </c>
+      <c r="E5" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F5" s="3">
+        <f t="shared" si="2"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" s="1">
+        <v>4</v>
+      </c>
+      <c r="C6" s="5">
+        <f t="shared" si="1"/>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="D6" s="5">
+        <f t="shared" si="0"/>
+        <v>4.4444444444444446E-2</v>
+      </c>
+      <c r="E6" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F6" s="3">
+        <f t="shared" si="2"/>
+        <v>8.8888888888888892E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" s="1">
+        <v>5</v>
+      </c>
+      <c r="C7" s="5">
+        <f t="shared" si="1"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="D7" s="5">
+        <f t="shared" si="0"/>
+        <v>5.5555555555555552E-2</v>
+      </c>
+      <c r="E7" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F7" s="3">
+        <f t="shared" si="2"/>
+        <v>0.1111111111111111</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" s="1">
+        <v>6</v>
+      </c>
+      <c r="C8" s="5">
+        <f t="shared" si="1"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="D8" s="5">
+        <f t="shared" si="0"/>
+        <v>6.6666666666666666E-2</v>
+      </c>
+      <c r="E8" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F8" s="3">
+        <f t="shared" si="2"/>
+        <v>0.13333333333333333</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" s="1">
+        <v>7</v>
+      </c>
+      <c r="C9" s="5">
+        <f t="shared" si="1"/>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="D9" s="5">
+        <f t="shared" si="0"/>
+        <v>7.7777777777777779E-2</v>
+      </c>
+      <c r="E9" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F9" s="3">
+        <f t="shared" si="2"/>
+        <v>0.15555555555555556</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" s="1">
+        <v>8</v>
+      </c>
+      <c r="C10" s="5">
+        <f t="shared" si="1"/>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="D10" s="5">
+        <f t="shared" si="0"/>
+        <v>8.8888888888888892E-2</v>
+      </c>
+      <c r="E10" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F10" s="3">
+        <f t="shared" si="2"/>
+        <v>0.17777777777777778</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" s="1">
+        <v>9</v>
+      </c>
+      <c r="C11" s="5">
+        <f t="shared" si="1"/>
+        <v>0.1</v>
+      </c>
+      <c r="D11" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="E11" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F11" s="3">
+        <f t="shared" si="2"/>
+        <v>0.2</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" s="1">
+        <v>10</v>
+      </c>
+      <c r="C12" s="5">
+        <f t="shared" si="1"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="D12" s="5">
+        <f t="shared" si="0"/>
+        <v>0.1111111111111111</v>
+      </c>
+      <c r="E12" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <f t="shared" si="2"/>
+        <v>0.22222222222222221</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" s="1">
+        <v>11</v>
+      </c>
+      <c r="C13" s="5">
+        <f t="shared" si="1"/>
+        <v>0.12222222222222222</v>
+      </c>
+      <c r="D13" s="5">
+        <f t="shared" si="0"/>
+        <v>0.12222222222222222</v>
+      </c>
+      <c r="E13" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F13" s="3">
+        <f t="shared" si="2"/>
+        <v>0.24444444444444444</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B14" s="1">
+        <v>12</v>
+      </c>
+      <c r="C14" s="5">
+        <f t="shared" si="1"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="D14" s="5">
+        <f t="shared" si="0"/>
+        <v>0.13333333333333333</v>
+      </c>
+      <c r="E14" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F14" s="3">
+        <f t="shared" si="2"/>
+        <v>0.26666666666666666</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B15" s="1">
+        <v>13</v>
+      </c>
+      <c r="C15" s="5">
+        <f t="shared" si="1"/>
+        <v>0.14444444444444443</v>
+      </c>
+      <c r="D15" s="5">
+        <f t="shared" si="0"/>
+        <v>0.14444444444444443</v>
+      </c>
+      <c r="E15" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F15" s="3">
+        <f t="shared" si="2"/>
+        <v>0.28888888888888886</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B16" s="1">
+        <v>14</v>
+      </c>
+      <c r="C16" s="5">
+        <f t="shared" si="1"/>
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="D16" s="5">
+        <f t="shared" si="0"/>
+        <v>0.15555555555555556</v>
+      </c>
+      <c r="E16" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F16" s="3">
+        <f t="shared" si="2"/>
+        <v>0.31111111111111112</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B17" s="1">
+        <v>15</v>
+      </c>
+      <c r="C17" s="5">
+        <f t="shared" si="1"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D17" s="5">
+        <f t="shared" si="0"/>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="E17" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F17" s="3">
+        <f t="shared" si="2"/>
+        <v>0.33333333333333331</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B18" s="1">
+        <v>16</v>
+      </c>
+      <c r="C18" s="5">
+        <f t="shared" si="1"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="D18" s="5">
+        <f t="shared" si="0"/>
+        <v>0.17777777777777778</v>
+      </c>
+      <c r="E18" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F18" s="3">
+        <f t="shared" si="2"/>
+        <v>0.35555555555555557</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B19" s="1">
+        <v>17</v>
+      </c>
+      <c r="C19" s="5">
+        <f t="shared" si="1"/>
+        <v>0.18888888888888888</v>
+      </c>
+      <c r="D19" s="5">
+        <f t="shared" si="0"/>
+        <v>0.18888888888888888</v>
+      </c>
+      <c r="E19" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F19" s="3">
+        <f t="shared" si="2"/>
+        <v>0.37777777777777777</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B20" s="1">
+        <v>18</v>
+      </c>
+      <c r="C20" s="5">
+        <f t="shared" si="1"/>
+        <v>0.2</v>
+      </c>
+      <c r="D20" s="5">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="E20" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F20" s="3">
+        <f t="shared" si="2"/>
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B21" s="1">
+        <v>19</v>
+      </c>
+      <c r="C21" s="5">
+        <f t="shared" si="1"/>
+        <v>0.21111111111111111</v>
+      </c>
+      <c r="D21" s="5">
+        <f t="shared" si="0"/>
+        <v>0.21111111111111111</v>
+      </c>
+      <c r="E21" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F21" s="3">
+        <f t="shared" si="2"/>
+        <v>0.42222222222222222</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B22" s="1">
+        <v>20</v>
+      </c>
+      <c r="C22" s="5">
+        <f t="shared" si="1"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D22" s="5">
+        <f t="shared" si="0"/>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="E22" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F22" s="3">
+        <f t="shared" si="2"/>
+        <v>0.44444444444444442</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B23" s="1">
+        <v>21</v>
+      </c>
+      <c r="C23" s="5">
+        <f t="shared" si="1"/>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="D23" s="5">
+        <f t="shared" si="0"/>
+        <v>0.23333333333333334</v>
+      </c>
+      <c r="E23" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F23" s="3">
+        <f t="shared" si="2"/>
+        <v>0.46666666666666667</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B24" s="1">
+        <v>22</v>
+      </c>
+      <c r="C24" s="5">
+        <f t="shared" si="1"/>
+        <v>0.24444444444444444</v>
+      </c>
+      <c r="D24" s="5">
+        <f t="shared" si="0"/>
+        <v>0.24444444444444444</v>
+      </c>
+      <c r="E24" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F24" s="3">
+        <f t="shared" si="2"/>
+        <v>0.48888888888888887</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B25" s="1">
+        <v>23</v>
+      </c>
+      <c r="C25" s="5">
+        <f t="shared" si="1"/>
+        <v>0.25555555555555554</v>
+      </c>
+      <c r="D25" s="5">
+        <f t="shared" si="0"/>
+        <v>0.25555555555555554</v>
+      </c>
+      <c r="E25" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F25" s="3">
+        <f t="shared" si="2"/>
+        <v>0.51111111111111107</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B26" s="1">
+        <v>24</v>
+      </c>
+      <c r="C26" s="5">
+        <f t="shared" si="1"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="D26" s="5">
+        <f t="shared" si="0"/>
+        <v>0.26666666666666666</v>
+      </c>
+      <c r="E26" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F26" s="3">
+        <f t="shared" si="2"/>
+        <v>0.53333333333333333</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B27" s="1">
+        <v>25</v>
+      </c>
+      <c r="C27" s="5">
+        <f t="shared" si="1"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="0"/>
+        <v>0.27777777777777779</v>
+      </c>
+      <c r="E27" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F27" s="3">
+        <f t="shared" si="2"/>
+        <v>0.55555555555555558</v>
+      </c>
+    </row>
+    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B28" s="1">
+        <v>26</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" si="1"/>
+        <v>0.28888888888888886</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="0"/>
+        <v>0.28888888888888886</v>
+      </c>
+      <c r="E28" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F28" s="3">
+        <f t="shared" si="2"/>
+        <v>0.57777777777777772</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B29" s="1">
+        <v>27</v>
+      </c>
+      <c r="C29" s="5">
+        <f t="shared" si="1"/>
+        <v>0.3</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="E29" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F29" s="3">
+        <f t="shared" si="2"/>
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B30" s="1">
+        <v>28</v>
+      </c>
+      <c r="C30" s="5">
+        <f t="shared" si="1"/>
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="0"/>
+        <v>0.31111111111111112</v>
+      </c>
+      <c r="E30" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F30" s="3">
+        <f t="shared" si="2"/>
+        <v>0.62222222222222223</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B31" s="1">
+        <v>29</v>
+      </c>
+      <c r="C31" s="5">
+        <f t="shared" si="1"/>
+        <v>0.32222222222222224</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="0"/>
+        <v>0.32222222222222224</v>
+      </c>
+      <c r="E31" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F31" s="3">
+        <f t="shared" si="2"/>
+        <v>0.64444444444444449</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B32" s="1">
+        <v>30</v>
+      </c>
+      <c r="C32" s="5">
+        <f t="shared" si="1"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="0"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="E32" s="3">
+        <v>0.33329999999999999</v>
+      </c>
+      <c r="F32" s="3">
+        <f t="shared" si="2"/>
+        <v>0.66666666666666663</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B33" s="1">
+        <v>31</v>
+      </c>
+      <c r="C33" s="5">
+        <f>30/90</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D33" s="5">
+        <f t="shared" si="0"/>
+        <v>0.34444444444444444</v>
+      </c>
+      <c r="E33" s="3">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="F33" s="3">
+        <f t="shared" si="2"/>
+        <v>0.67777777777777781</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B34" s="1">
+        <v>32</v>
+      </c>
+      <c r="C34" s="5">
+        <f t="shared" ref="C34:C62" si="3">30/90</f>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D34" s="5">
+        <f t="shared" si="0"/>
+        <v>0.35555555555555557</v>
+      </c>
+      <c r="E34" s="3">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="F34" s="3">
+        <f t="shared" si="2"/>
+        <v>0.68888888888888888</v>
+      </c>
+    </row>
+    <row r="35" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B35" s="1">
+        <v>33</v>
+      </c>
+      <c r="C35" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D35" s="5">
+        <f t="shared" si="0"/>
+        <v>0.36666666666666664</v>
+      </c>
+      <c r="E35" s="3">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="F35" s="3">
+        <f t="shared" si="2"/>
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="36" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B36" s="1">
+        <v>34</v>
+      </c>
+      <c r="C36" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D36" s="5">
+        <f t="shared" si="0"/>
+        <v>0.37777777777777777</v>
+      </c>
+      <c r="E36" s="3">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="F36" s="3">
+        <f t="shared" si="2"/>
+        <v>0.71111111111111103</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B37" s="1">
+        <v>35</v>
+      </c>
+      <c r="C37" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D37" s="5">
+        <f t="shared" si="0"/>
+        <v>0.3888888888888889</v>
+      </c>
+      <c r="E37" s="3">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="F37" s="3">
+        <f t="shared" si="2"/>
+        <v>0.72222222222222221</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B38" s="1">
+        <v>36</v>
+      </c>
+      <c r="C38" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D38" s="5">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="E38" s="3">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="F38" s="3">
+        <f t="shared" si="2"/>
+        <v>0.73333333333333339</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B39" s="1">
+        <v>37</v>
+      </c>
+      <c r="C39" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D39" s="5">
+        <f t="shared" si="0"/>
+        <v>0.41111111111111109</v>
+      </c>
+      <c r="E39" s="3">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="F39" s="3">
+        <f t="shared" si="2"/>
+        <v>0.74444444444444446</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B40" s="1">
+        <v>38</v>
+      </c>
+      <c r="C40" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D40" s="5">
+        <f t="shared" si="0"/>
+        <v>0.42222222222222222</v>
+      </c>
+      <c r="E40" s="3">
+        <v>0.42220000000000002</v>
+      </c>
+      <c r="F40" s="3">
+        <f t="shared" si="2"/>
+        <v>0.75555555555555554</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B41" s="1">
+        <v>39</v>
+      </c>
+      <c r="C41" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D41" s="5">
+        <f t="shared" si="0"/>
+        <v>0.43333333333333335</v>
+      </c>
+      <c r="E41" s="3">
+        <v>1</v>
+      </c>
+      <c r="F41" s="3">
+        <f t="shared" si="2"/>
+        <v>0.76666666666666661</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B42" s="1">
+        <v>40</v>
+      </c>
+      <c r="C42" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D42" s="5">
+        <f t="shared" si="0"/>
+        <v>0.44444444444444442</v>
+      </c>
+      <c r="E42" s="3">
+        <v>1</v>
+      </c>
+      <c r="F42" s="3">
+        <f t="shared" si="2"/>
+        <v>0.77777777777777768</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B43" s="1">
+        <v>41</v>
+      </c>
+      <c r="C43" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D43" s="5">
+        <f t="shared" si="0"/>
+        <v>0.45555555555555555</v>
+      </c>
+      <c r="E43" s="3">
+        <v>1</v>
+      </c>
+      <c r="F43" s="3">
+        <f t="shared" si="2"/>
+        <v>0.78888888888888886</v>
+      </c>
+    </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B44" s="1">
+        <v>42</v>
+      </c>
+      <c r="C44" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D44" s="5">
+        <f t="shared" si="0"/>
+        <v>0.46666666666666667</v>
+      </c>
+      <c r="E44" s="3">
+        <v>1</v>
+      </c>
+      <c r="F44" s="3">
+        <f t="shared" si="2"/>
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B45" s="1">
+        <v>43</v>
+      </c>
+      <c r="C45" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D45" s="5">
+        <f t="shared" si="0"/>
+        <v>0.4777777777777778</v>
+      </c>
+      <c r="E45" s="3">
+        <v>1</v>
+      </c>
+      <c r="F45" s="3">
+        <f t="shared" si="2"/>
+        <v>0.81111111111111112</v>
+      </c>
+    </row>
+    <row r="46" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B46" s="1">
+        <v>44</v>
+      </c>
+      <c r="C46" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D46" s="5">
+        <f t="shared" si="0"/>
+        <v>0.48888888888888887</v>
+      </c>
+      <c r="E46" s="3">
+        <v>1</v>
+      </c>
+      <c r="F46" s="3">
+        <f t="shared" si="2"/>
+        <v>0.82222222222222219</v>
+      </c>
+    </row>
+    <row r="47" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B47" s="1">
+        <v>45</v>
+      </c>
+      <c r="C47" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D47" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5</v>
+      </c>
+      <c r="E47" s="3">
+        <v>1</v>
+      </c>
+      <c r="F47" s="3">
+        <f t="shared" si="2"/>
+        <v>0.83333333333333326</v>
+      </c>
+    </row>
+    <row r="48" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B48" s="1">
+        <v>46</v>
+      </c>
+      <c r="C48" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D48" s="5">
+        <f t="shared" si="0"/>
+        <v>0.51111111111111107</v>
+      </c>
+      <c r="E48" s="3">
+        <v>1</v>
+      </c>
+      <c r="F48" s="3">
+        <f t="shared" si="2"/>
+        <v>0.84444444444444433</v>
+      </c>
+    </row>
+    <row r="49" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B49" s="1">
+        <v>47</v>
+      </c>
+      <c r="C49" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D49" s="5">
+        <f t="shared" si="0"/>
+        <v>0.52222222222222225</v>
+      </c>
+      <c r="E49" s="3">
+        <v>1</v>
+      </c>
+      <c r="F49" s="3">
+        <f t="shared" si="2"/>
+        <v>0.85555555555555562</v>
+      </c>
+    </row>
+    <row r="50" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B50" s="1">
+        <v>48</v>
+      </c>
+      <c r="C50" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D50" s="5">
+        <f t="shared" si="0"/>
+        <v>0.53333333333333333</v>
+      </c>
+      <c r="E50" s="3">
+        <v>1</v>
+      </c>
+      <c r="F50" s="3">
+        <f t="shared" si="2"/>
+        <v>0.8666666666666667</v>
+      </c>
+    </row>
+    <row r="51" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B51" s="1">
+        <v>49</v>
+      </c>
+      <c r="C51" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D51" s="5">
+        <f t="shared" si="0"/>
+        <v>0.5444444444444444</v>
+      </c>
+      <c r="E51" s="3">
+        <v>1</v>
+      </c>
+      <c r="F51" s="3">
+        <f t="shared" si="2"/>
+        <v>0.87777777777777777</v>
+      </c>
+    </row>
+    <row r="52" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B52" s="1">
+        <v>50</v>
+      </c>
+      <c r="C52" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D52" s="5">
+        <f t="shared" si="0"/>
+        <v>0.55555555555555558</v>
+      </c>
+      <c r="E52" s="3">
+        <v>1</v>
+      </c>
+      <c r="F52" s="3">
+        <f t="shared" si="2"/>
+        <v>0.88888888888888884</v>
+      </c>
+    </row>
+    <row r="53" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B53" s="1">
+        <v>51</v>
+      </c>
+      <c r="C53" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D53" s="5">
+        <f t="shared" si="0"/>
+        <v>0.56666666666666665</v>
+      </c>
+      <c r="E53" s="3">
+        <v>1</v>
+      </c>
+      <c r="F53" s="3">
+        <f t="shared" si="2"/>
+        <v>0.89999999999999991</v>
+      </c>
+    </row>
+    <row r="54" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B54" s="1">
+        <v>52</v>
+      </c>
+      <c r="C54" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D54" s="5">
+        <f t="shared" si="0"/>
+        <v>0.57777777777777772</v>
+      </c>
+      <c r="E54" s="3">
+        <v>1</v>
+      </c>
+      <c r="F54" s="3">
+        <f t="shared" si="2"/>
+        <v>0.91111111111111098</v>
+      </c>
+    </row>
+    <row r="55" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B55" s="1">
+        <v>53</v>
+      </c>
+      <c r="C55" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D55" s="5">
+        <f t="shared" si="0"/>
+        <v>0.58888888888888891</v>
+      </c>
+      <c r="E55" s="3">
+        <v>1</v>
+      </c>
+      <c r="F55" s="3">
+        <f t="shared" si="2"/>
+        <v>0.92222222222222228</v>
+      </c>
+    </row>
+    <row r="56" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B56" s="1">
+        <v>54</v>
+      </c>
+      <c r="C56" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D56" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6</v>
+      </c>
+      <c r="E56" s="3">
+        <v>1</v>
+      </c>
+      <c r="F56" s="3">
+        <f t="shared" si="2"/>
+        <v>0.93333333333333335</v>
+      </c>
+    </row>
+    <row r="57" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B57" s="1">
+        <v>55</v>
+      </c>
+      <c r="C57" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D57" s="5">
+        <f t="shared" si="0"/>
+        <v>0.61111111111111116</v>
+      </c>
+      <c r="E57" s="3">
+        <v>1</v>
+      </c>
+      <c r="F57" s="3">
+        <f t="shared" si="2"/>
+        <v>0.94444444444444442</v>
+      </c>
+    </row>
+    <row r="58" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B58" s="1">
+        <v>56</v>
+      </c>
+      <c r="C58" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D58" s="5">
+        <f t="shared" si="0"/>
+        <v>0.62222222222222223</v>
+      </c>
+      <c r="E58" s="3">
+        <v>1</v>
+      </c>
+      <c r="F58" s="3">
+        <f t="shared" si="2"/>
+        <v>0.95555555555555549</v>
+      </c>
+    </row>
+    <row r="59" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B59" s="1">
+        <v>57</v>
+      </c>
+      <c r="C59" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D59" s="5">
+        <f t="shared" si="0"/>
+        <v>0.6333333333333333</v>
+      </c>
+      <c r="E59" s="3">
+        <v>1</v>
+      </c>
+      <c r="F59" s="3">
+        <f t="shared" si="2"/>
+        <v>0.96666666666666656</v>
+      </c>
+    </row>
+    <row r="60" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B60" s="1">
+        <v>58</v>
+      </c>
+      <c r="C60" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D60" s="5">
+        <f t="shared" si="0"/>
+        <v>0.64444444444444449</v>
+      </c>
+      <c r="E60" s="3">
+        <v>1</v>
+      </c>
+      <c r="F60" s="3">
+        <f t="shared" si="2"/>
+        <v>0.97777777777777786</v>
+      </c>
+    </row>
+    <row r="61" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B61" s="1">
+        <v>59</v>
+      </c>
+      <c r="C61" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D61" s="5">
+        <f t="shared" si="0"/>
+        <v>0.65555555555555556</v>
+      </c>
+      <c r="E61" s="3">
+        <v>1</v>
+      </c>
+      <c r="F61" s="3">
+        <f t="shared" si="2"/>
+        <v>0.98888888888888893</v>
+      </c>
+    </row>
+    <row r="62" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B62" s="1">
+        <v>60</v>
+      </c>
+      <c r="C62" s="5">
+        <f t="shared" si="3"/>
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D62" s="5">
+        <f t="shared" si="0"/>
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="E62" s="3">
+        <v>1</v>
+      </c>
+      <c r="F62" s="3">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
 </file>
</xml_diff>